<commit_message>
Add dependency injection extensions.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ReturnProtocol.xlsx
+++ b/DayReportsDataBase/ExportFiles/ReturnProtocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\source\repos\DelitaTrade\DayReportsDataBase\ExportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48216E8E-A839-4EB5-8888-B3B4CB561930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D240AC57-A9A9-4371-AC3C-4C4328DDA167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -1214,7 +1214,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA1E1C2-31D8-3F1D-EBD7-E12AFB0A54E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{305B0833-2938-AA9F-EDA8-068DFFA68E5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1264,7 +1264,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4115E231-82C0-2A7A-992A-76717BCD783D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E235C533-94AB-4684-6C0E-D6121807325A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1314,7 +1314,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F77F12-8E8E-9663-CAD8-4FFD717866C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB8CB64F-AD73-6EEF-20BE-CD5F03165207}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1364,7 +1364,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9EB2A40-2DF0-474A-955C-2F1208A0C0A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7251F8-CB2F-1148-D34E-69DC1B4D1617}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1414,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9030BCF6-8F3E-BDAF-B05A-447C9BEEBD8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F741190-7938-6B42-B75E-4918B39E5FBC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1464,7 +1464,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68FD3AE6-85F5-D57B-73E0-B8A3A44495F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD603B1D-E0F3-A747-5411-9DD46933247A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>